<commit_message>
k78, 79, 80, k177, 178, 179, 180
</commit_message>
<xml_diff>
--- a/cnttcb/lichhoc-3-2023.xlsx
+++ b/cnttcb/lichhoc-3-2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\learn\cnttcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D1A7EE-8623-46D4-8ADA-DAA57D74EB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C9E1CE-D797-4176-81FC-DDFA06191C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{EFE87E7B-E890-42A1-8399-625B02850241}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E12" sqref="E11:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +683,7 @@
         <v>44985</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -712,7 +712,7 @@
         <v>45063</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -770,7 +770,7 @@
         <v>45066</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -799,7 +799,7 @@
         <v>45043</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -828,7 +828,7 @@
         <v>45036</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -857,7 +857,7 @@
         <v>45035</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -886,7 +886,7 @@
         <v>45051</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -915,7 +915,7 @@
         <v>45016</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -944,7 +944,7 @@
         <v>45026</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>45030</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>45060</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>45012</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1325,15 +1325,17 @@
   <autoFilter ref="A1:J24" xr:uid="{66BF367C-58DF-427A-BF24-B318B00C9CD6}">
     <filterColumn colId="5">
       <filters>
+        <filter val="Tối 2-4-6"/>
         <filter val="Tối 3-4-5"/>
-        <filter val="Tối 3-5-7"/>
-        <filter val="Tối T3-5 và Sáng T7"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="7">
+    <filterColumn colId="8">
       <filters>
-        <dateGroupItem year="2023" month="2" dateTimeGrouping="month"/>
-        <dateGroupItem year="2023" month="3" dateTimeGrouping="month"/>
+        <dateGroupItem year="2023" month="3" day="27" dateTimeGrouping="day"/>
+        <dateGroupItem year="2023" month="3" day="28" dateTimeGrouping="day"/>
+        <dateGroupItem year="2023" month="3" day="31" dateTimeGrouping="day"/>
+        <dateGroupItem year="2023" month="4" dateTimeGrouping="month"/>
+        <dateGroupItem year="2023" month="5" dateTimeGrouping="month"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>